<commit_message>
Updated the model calculation algorithm. Improved performance. Updated saving to file.
</commit_message>
<xml_diff>
--- a/DATA/reactor/Mol_Reactor.xlsx
+++ b/DATA/reactor/Mol_Reactor.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Models_In_Python\Work_Model v4.0\DATA\reactor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41883557-F0E0-4560-BF3C-83AE99AC1456}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CDE2E1A-7936-4590-A880-55AAD29E0E63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>№</t>
   </si>
@@ -52,9 +52,6 @@
   </si>
   <si>
     <t>steps</t>
-  </si>
-  <si>
-    <t>molar_flow_in</t>
   </si>
 </sst>
 </file>
@@ -380,7 +377,7 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -421,9 +418,6 @@
       <c r="H1" t="s">
         <v>8</v>
       </c>
-      <c r="I1" t="s">
-        <v>9</v>
-      </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
@@ -450,9 +444,7 @@
       <c r="H2" s="2">
         <v>10000</v>
       </c>
-      <c r="I2" s="1">
-        <v>10</v>
-      </c>
+      <c r="I2" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>